<commit_message>
reorganized case studies; changed end date for WTI; using standardized f for WTI and for stock (instead of only for stock)
</commit_message>
<xml_diff>
--- a/case-2/data/factor_calibrations.xlsx
+++ b/case-2/data/factor_calibrations.xlsx
@@ -436,7 +436,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.0008887854659561153</v>
+        <v>0.008517853992011859</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -444,7 +444,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.7727922900322718</v>
+        <v>0.7574397510546335</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -452,7 +452,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.1005288770640802</v>
+        <v>0.1449643810992358</v>
       </c>
     </row>
   </sheetData>
@@ -478,7 +478,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>-0.09306512800291195</v>
+        <v>-0.1924922941771267</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -486,7 +486,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.729940048388102</v>
+        <v>0.5489540365738861</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -494,7 +494,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.07780760966866578</v>
+        <v>0.1056995749862125</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -502,7 +502,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.09573379536244561</v>
+        <v>0.1989364521800432</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -510,7 +510,7 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.6962706411279245</v>
+        <v>0.5554828186427432</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -518,7 +518,7 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>0.06103817075380358</v>
+        <v>0.1022394987945887</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-0.0009891166833161688</v>
+        <v>0.0008216282642889191</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -560,7 +560,7 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>0.002268313855635574</v>
+        <v>0.125904208037552</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -568,7 +568,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.1999993330331042</v>
+        <v>0.1036620094463338</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -576,7 +576,7 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>0.7800007428514291</v>
+        <v>0.1210785535428306</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +602,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-0.001065093801448775</v>
+        <v>-0.0006789516040753972</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -610,7 +610,7 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>0.002269123102064011</v>
+        <v>0.1275789815885949</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -618,7 +618,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.1999995091724977</v>
+        <v>0.08307317486530481</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -626,7 +626,7 @@
         <v>14</v>
       </c>
       <c r="B5">
-        <v>0.00999997185428371</v>
+        <v>0.03876898703901042</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -634,7 +634,7 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>0.7750005422751267</v>
+        <v>0.1114728437573284</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -668,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.001706453550795025</v>
+        <v>0.00935930655650029</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -676,7 +676,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.7760529830641222</v>
+        <v>0.7573059024682156</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -684,7 +684,7 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>0.002010370423522397</v>
+        <v>0.1289823215569525</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -692,7 +692,7 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>0.199979546336019</v>
+        <v>0.07188003838808588</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>0.009999039529196617</v>
+        <v>0.05942438202419818</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -708,7 +708,7 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0.775023178175507</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">

</xml_diff>